<commit_message>
Fix broken URL issue
</commit_message>
<xml_diff>
--- a/en/docs/assets/docs/vulnerability-report-template_public.xlsx
+++ b/en/docs/assets/docs/vulnerability-report-template_public.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t>title</t>
   </si>
@@ -66,16 +66,16 @@
     <t>scanner_report_type</t>
   </si>
   <si>
-    <t>[note] WSO2 Resolution_1</t>
-  </si>
-  <si>
-    <t>[note] Use Case_1</t>
-  </si>
-  <si>
-    <t>[note] Vulnerability Influence_1</t>
-  </si>
-  <si>
-    <t>[note] Resolution_1</t>
+    <t>[note] wso2-resolution</t>
+  </si>
+  <si>
+    <t>[note] usecase</t>
+  </si>
+  <si>
+    <t>[note] justification</t>
+  </si>
+  <si>
+    <t>[note] resolution</t>
   </si>
   <si>
     <t>CVE-2013-0248 Commons-Fileupload:commons-Fileupload 1.2.1</t>
@@ -160,7 +160,7 @@
     <t>Dynamic</t>
   </si>
   <si>
-    <t>[note] WSO2 Resolution_1:</t>
+    <t xml:space="preserve">[note] wso2-resolution : </t>
   </si>
   <si>
     <t>WSO2 Resolution can be categorized into the following six types.</t>
@@ -183,7 +183,8 @@
   </si>
   <si>
     <t>Issue is valid from scanner's point of view, but does not pose a threat in WSO2 product's context.
-(Ex:Vulnerable class or method not used in the product, misconfiguration on users' end)</t>
+(Ex:Vulnerable class or method not used in the product, misconfiguration on users' end)
+For third-party dependency issues this should be used only if it is not possible to update the dependency due to a major/architectural change required blocking the update.</t>
   </si>
   <si>
     <t>Need to Fix</t>
@@ -192,10 +193,26 @@
     <t>Issue exists, and needs to be fixed. (True Positive)</t>
   </si>
   <si>
-    <t>Already Mitigated</t>
-  </si>
-  <si>
-    <t>Issues which can be mitigated by existing patches, configuration changes or workarounds.</t>
+    <t>Batch for Patching</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">Only applicable for third-party dependencies.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>Vulnerability does not affect the security of the product. However, have been batch for dependency upgrade, migrate, or removal to prevent scanner detections.</t>
+    </r>
   </si>
   <si>
     <t>Not Applicable</t>
@@ -211,19 +228,25 @@
     <t>Scan report (specially externally provided report) does not contain enough information about the vulnerability in order to come to a proper conclusion about the vulnerability.</t>
   </si>
   <si>
-    <t xml:space="preserve">[note] Use Case_1: </t>
+    <t>Already Mitigated</t>
+  </si>
+  <si>
+    <t>Issues which can be mitigated by existing patches, configuration changes or workarounds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[note] usecase : </t>
   </si>
   <si>
     <t>This field gives a brief summary of the use case of the reported method/ class/ URL path/ web page to the product.</t>
   </si>
   <si>
-    <t>[note] Vulnerability Influence_1:</t>
+    <t>[note] justification :</t>
   </si>
   <si>
     <t>This is a summary explaining how the vulnerability affects or not affects the product (Justification for the value selected for WSO2 Resolution).</t>
   </si>
   <si>
-    <t>[note] Resolution_1:</t>
+    <t>[note] resolution :</t>
   </si>
   <si>
     <t>This field proposed the solution to fix or mitigate the vulnerability.</t>
@@ -313,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -328,9 +351,6 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
@@ -375,7 +395,19 @@
     <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,62 +706,62 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2">
-      <c r="D2" s="7"/>
-      <c r="Q2" s="8"/>
+      <c r="D2" s="6"/>
+      <c r="Q2" s="7"/>
     </row>
     <row r="3">
-      <c r="D3" s="7"/>
-      <c r="Q3" s="8"/>
+      <c r="D3" s="6"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4">
-      <c r="D4" s="7"/>
-      <c r="Q4" s="8"/>
+      <c r="D4" s="6"/>
+      <c r="Q4" s="7"/>
     </row>
     <row r="5">
-      <c r="D5" s="7"/>
-      <c r="Q5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="Q5" s="7"/>
     </row>
     <row r="6">
-      <c r="D6" s="7"/>
-      <c r="Q6" s="8"/>
+      <c r="D6" s="6"/>
+      <c r="Q6" s="7"/>
     </row>
     <row r="7">
-      <c r="D7" s="7"/>
-      <c r="Q7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="Q7" s="7"/>
     </row>
     <row r="8">
-      <c r="D8" s="7"/>
-      <c r="Q8" s="8"/>
+      <c r="D8" s="6"/>
+      <c r="Q8" s="7"/>
     </row>
     <row r="9">
-      <c r="D9" s="7"/>
-      <c r="Q9" s="8"/>
+      <c r="D9" s="6"/>
+      <c r="Q9" s="7"/>
     </row>
     <row r="10">
-      <c r="D10" s="7"/>
-      <c r="Q10" s="8"/>
+      <c r="D10" s="6"/>
+      <c r="Q10" s="7"/>
     </row>
     <row r="11">
-      <c r="D11" s="7"/>
-      <c r="Q11" s="8"/>
+      <c r="D11" s="6"/>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12">
-      <c r="D12" s="7"/>
-      <c r="Q12" s="8"/>
+      <c r="D12" s="6"/>
+      <c r="Q12" s="7"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -787,7 +819,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -802,7 +834,7 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -811,7 +843,7 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -826,156 +858,156 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>102.0</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="14"/>
-      <c r="H2" s="12" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="13"/>
+      <c r="H2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="Q2" s="16" t="s">
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="Q2" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3">
-      <c r="D3" s="7"/>
-      <c r="E3" s="14"/>
-      <c r="I3" s="12" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="13"/>
+      <c r="I3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="Q3" s="16" t="s">
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="Q3" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4">
-      <c r="D4" s="7"/>
-      <c r="E4" s="14"/>
-      <c r="I4" s="8" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="13"/>
+      <c r="I4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="Q4" s="16" t="s">
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="Q4" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5">
-      <c r="D5" s="7"/>
-      <c r="E5" s="14"/>
-      <c r="I5" s="12" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="13"/>
+      <c r="I5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="14"/>
-      <c r="Q5" s="16" t="s">
+      <c r="N5" s="13"/>
+      <c r="Q5" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>98.0</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="14"/>
-      <c r="J6" s="15" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="13"/>
+      <c r="J6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12" t="s">
+      <c r="K6" s="11"/>
+      <c r="L6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="14"/>
-      <c r="Q6" s="16" t="s">
+      <c r="N6" s="13"/>
+      <c r="Q6" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>202.0</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="M7" s="17" t="s">
+      <c r="J7" s="13"/>
+      <c r="M7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="17">
         <v>54.0</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="15" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1005,24 +1037,25 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="28.75"/>
     <col customWidth="1" min="2" max="2" width="26.63"/>
-    <col customWidth="1" min="3" max="3" width="77.38"/>
+    <col customWidth="1" min="3" max="4" width="77.38"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>49</v>
       </c>
+      <c r="D4" s="20"/>
     </row>
     <row r="5">
       <c r="B5" s="21" t="s">
@@ -1031,6 +1064,7 @@
       <c r="C5" s="21" t="s">
         <v>51</v>
       </c>
+      <c r="D5" s="22"/>
     </row>
     <row r="6">
       <c r="B6" s="21" t="s">
@@ -1039,6 +1073,7 @@
       <c r="C6" s="21" t="s">
         <v>53</v>
       </c>
+      <c r="D6" s="22"/>
     </row>
     <row r="7">
       <c r="B7" s="21" t="s">
@@ -1047,14 +1082,16 @@
       <c r="C7" s="21" t="s">
         <v>55</v>
       </c>
+      <c r="D7" s="22"/>
     </row>
     <row r="8">
       <c r="B8" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="23" t="s">
         <v>57</v>
       </c>
+      <c r="D8" s="24"/>
     </row>
     <row r="9">
       <c r="B9" s="21" t="s">
@@ -1063,6 +1100,7 @@
       <c r="C9" s="21" t="s">
         <v>59</v>
       </c>
+      <c r="D9" s="22"/>
     </row>
     <row r="10">
       <c r="B10" s="21" t="s">
@@ -1071,29 +1109,39 @@
       <c r="C10" s="21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="19" t="s">
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C11" s="21" t="s">
         <v>63</v>
       </c>
+      <c r="D11" s="22"/>
     </row>
     <row r="14">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>